<commit_message>
fixed steam reforming elc/lng ratio, hydrogen seasonal storage
Former-commit-id: 765046bc6cc6a3bddeba0f18275b89d5f81a8ce6
Former-commit-id: 734fe465713707cc0473439c3df205f05812f6f2
</commit_message>
<xml_diff>
--- a/data/elecgen/elecsup-genutils-monthly-1986-750100-e.xlsx
+++ b/data/elecgen/elecsup-genutils-monthly-1986-750100-e.xlsx
@@ -1,15 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\i2cner\data\elecgen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281BC6B3-CE84-46AD-B71A-D52B2F53CB60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="660" windowWidth="27555" windowHeight="11985"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -120,11 +134,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="mm/yyyy"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -187,13 +201,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
@@ -202,21 +216,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -258,7 +280,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +312,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +364,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,35 +557,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S382"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B352" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="M379" sqref="M379"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -559,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" ht="89.25">
+    <row r="6" spans="1:19" s="3" customFormat="1" ht="82.8">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -17989,6 +18047,22 @@
       <c r="R376" s="7"/>
       <c r="S376" s="7"/>
     </row>
+    <row r="377" spans="1:19">
+      <c r="C377" s="7">
+        <f>SUM(C362:C373)</f>
+        <v>63906732</v>
+      </c>
+      <c r="M377" s="7">
+        <f>SUM(M362:M373)</f>
+        <v>-5321526</v>
+      </c>
+    </row>
+    <row r="378" spans="1:19">
+      <c r="M378">
+        <f>M377/C377</f>
+        <v>-8.3270194445242487E-2</v>
+      </c>
+    </row>
     <row r="379" spans="1:19">
       <c r="A379" t="s">
         <v>24</v>
@@ -18012,7 +18086,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="F1" location="Sheet1!A379" display="To notes"/>
+    <hyperlink ref="F1" location="Sheet1!A379" display="To notes" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>